<commit_message>
Latest delivery of ID-1006 on 25052021
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="3" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>UI development</t>
   </si>
@@ -71,6 +66,39 @@
 CRUD operation for Saas Parameter.</t>
   </si>
   <si>
+    <t>SQL Task</t>
+  </si>
+  <si>
+    <t>SAAS customer DB Download</t>
+  </si>
+  <si>
+    <t>1)List Customer Databases 
+2) Download functionality of Backup 
+3) Upload functionality 
+4) Application parameter settings for downlaod and upload size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As per discussion tested file limit for download/upload  - 1GB </t>
+  </si>
+  <si>
+    <t>Add Other Settings and Sort discovery methods</t>
+  </si>
+  <si>
+    <t>1) add other settings to 3rd party intigrations
+2) disable buttons 
+3) add sorting functionality for discovery methods
+4) save sorting order of discovery methods</t>
+  </si>
+  <si>
+    <t>Saas Server Configuration</t>
+  </si>
+  <si>
+    <t>1) Created API to check Server is configured or not
+2) made UI changes to call the API
+3) changed UI to call Prashant's API
+4) Worked on feedback points given by gopichand</t>
+  </si>
+  <si>
     <t>SQL development</t>
   </si>
   <si>
@@ -89,26 +117,33 @@
     <t>Created the Create, Update, Delete records Sps and Get record(s) Sp of NZInfo Table in NzSaas Database</t>
   </si>
   <si>
-    <t>27/04/2021</t>
-  </si>
-  <si>
     <t>Saas Project JOB</t>
   </si>
   <si>
-    <t>29/04/2021</t>
-  </si>
-  <si>
     <t>Created Table to store SaasCustomerledger, Created Sp to get and insert customer rack,user and site count from their respective database into the Saas DB table. Schedule a Job to perform the action daily at 2:00:00 PM</t>
+  </si>
+  <si>
+    <t>Created required Stored Procedures , Functions, Type in NzEnt and NzSaas Database for the Upload and Download DataBase functionality.
+CONFIG_spCreateBackUpAndGetData
+CONFIG_spSaveBakFile</t>
+  </si>
+  <si>
+    <t>1) Created API for Restoring NzSaas Database (4 methods - 1 in SaasService.svc.cs and 3 in NzServermangerment..cs)
+2) Added new DataSource column to SAAS.instances table and updated Stored Procedure(SAAS_spSetServerInstanceForSaas) to Add/Update DataSource column value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +158,159 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +323,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -146,34 +518,321 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -431,34 +1090,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.42592592592593" customWidth="1"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="40.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="17.287037037037" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7109375" customWidth="1"/>
+    <col min="6" max="7" width="10.287037037037" customWidth="1"/>
+    <col min="9" max="9" width="53.8611111111111" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -486,21 +1146,21 @@
         <v>7</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" ht="43.2" spans="1:10">
       <c r="A4">
         <v>1001</v>
       </c>
       <c r="B4" s="4">
         <v>44287</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
@@ -516,7 +1176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="60">
+    <row r="5" ht="57.6" spans="1:9">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -536,57 +1196,111 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1003</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="57.6" spans="1:10">
       <c r="A7">
         <v>1004</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="B7" s="4">
+        <v>44316</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44326</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="57.6" spans="1:9">
       <c r="A8">
         <v>1005</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="B8" s="4">
+        <v>44329</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44331</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="57.6" spans="1:9">
       <c r="A9">
         <v>1006</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="B9" s="4">
+        <v>44335</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4">
+        <v>44336</v>
+      </c>
+      <c r="F9" s="4">
+        <v>44341</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10">
         <v>1007</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:1">
       <c r="A11">
         <v>1008</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:1">
       <c r="A12">
         <v>1009</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:1">
       <c r="A13">
         <v>1010</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:1">
       <c r="A14">
         <v>1011</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:1">
       <c r="A15">
         <v>1012</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:1">
       <c r="A16">
         <v>1013</v>
       </c>
@@ -648,33 +1362,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.42592592592593" customWidth="1"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="51.1388888888889" customWidth="1"/>
+    <col min="4" max="4" width="16.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="19.4259259259259" customWidth="1"/>
+    <col min="6" max="7" width="10.287037037037" customWidth="1"/>
+    <col min="9" max="9" width="53.8611111111111" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -700,14 +1416,14 @@
         <v>7</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="75">
+    <row r="4" ht="72" spans="1:10">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -715,22 +1431,22 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" ht="28.8" spans="1:9">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -738,84 +1454,117 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" ht="57.6" spans="1:9">
       <c r="A6">
         <v>1003</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
+      <c r="B6" s="4">
+        <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" ht="72" spans="1:9">
       <c r="A7">
         <v>1004</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="B7" s="4">
+        <v>44316</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44326</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8">
         <v>1005</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" ht="72" spans="1:9">
       <c r="A9">
         <v>1006</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="B9" s="4">
+        <v>44329</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4">
+        <v>44336</v>
+      </c>
+      <c r="F9" s="4">
+        <v>44341</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10">
         <v>1007</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:1">
       <c r="A11">
         <v>1008</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:1">
       <c r="A12">
         <v>1009</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:1">
       <c r="A13">
         <v>1010</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:1">
       <c r="A14">
         <v>1011</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:1">
       <c r="A15">
         <v>1012</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:1">
       <c r="A16">
         <v>1013</v>
       </c>
@@ -877,5 +1626,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Delivery note modified with 1006 update and 1007 as new Task Recording added for review of task 1006
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>UI development</t>
   </si>
@@ -96,7 +96,17 @@
     <t>1) Created API to check Server is configured or not
 2) made UI changes to call the API
 3) changed UI to call Prashant's API
-4) Worked on feedback points given by gopichand</t>
+4) Worked on feedback points given by gopichand
+5) Created Container form with name Saas_Server_Container
+6) Changed UI using newly created form</t>
+  </si>
+  <si>
+    <t>Property Grid tooltip styling</t>
+  </si>
+  <si>
+    <t>1) changed default tooltip with custom tooltip
+2) checked all form location where property grid is used
+3) updated new CSS in style.override.css file for common use</t>
   </si>
   <si>
     <t>SQL development</t>
@@ -130,6 +140,9 @@
   <si>
     <t>1) Created API for Restoring NzSaas Database (4 methods - 1 in SaasService.svc.cs and 3 in NzServermangerment..cs)
 2) Added new DataSource column to SAAS.instances table and updated Stored Procedure(SAAS_spSetServerInstanceForSaas) to Add/Update DataSource column value</t>
+  </si>
+  <si>
+    <t>UI-task</t>
   </si>
 </sst>
 </file>
@@ -137,11 +150,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -166,6 +179,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -180,11 +201,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,38 +248,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -251,52 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,6 +284,44 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -325,91 +338,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,91 +518,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,8 +535,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,7 +545,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,6 +576,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,30 +621,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -601,166 +629,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -771,7 +784,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1098,12 +1111,12 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1247,7 +1260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="57.6" spans="1:9">
+    <row r="9" ht="86.4" spans="1:9">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -1266,13 +1279,31 @@
       <c r="F9" s="4">
         <v>44341</v>
       </c>
+      <c r="G9" s="4">
+        <v>44344</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" ht="43.2" spans="1:9">
       <c r="A10">
         <v>1007</v>
+      </c>
+      <c r="B10" s="4">
+        <v>44342</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4">
+        <v>44344</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -1372,8 +1403,8 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1390,7 +1421,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1431,16 +1462,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1454,16 +1485,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1474,16 +1505,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1497,13 +1528,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1522,7 +1553,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1531,12 +1562,15 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>1007</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1">

</xml_diff>

<commit_message>
Task update 1008 - Grid Extender-control enhancement
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>UI development</t>
   </si>
@@ -109,6 +109,39 @@
 3) updated new CSS in style.override.css file for common use</t>
   </si>
   <si>
+    <t>Grid Extender-control enhancement</t>
+  </si>
+  <si>
+    <t>1) Hide Column,Sort column,Move column,tooltip on column
+2) Get and Set Column width and order
+3) Export and Delete and Edit function 
+4) Working on dynamic pagination as discussed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reoderable,Tooltip,Export,Delete and Edit columnMenu properties and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Events like reorderColumn,resizeColumn,remove,save and dataBinding</t>
+    </r>
+  </si>
+  <si>
     <t>SQL development</t>
   </si>
   <si>
@@ -143,6 +176,9 @@
   </si>
   <si>
     <t>UI-task</t>
+  </si>
+  <si>
+    <t>Added 7 Column in NZ.ValueByName Table and updated the 2 Sps to insert and update the column Values</t>
   </si>
 </sst>
 </file>
@@ -150,13 +186,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,62 +215,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,6 +260,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -257,67 +307,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,13 +380,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,31 +464,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,127 +554,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,11 +574,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,30 +623,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -600,6 +633,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,161 +677,167 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,12 +1159,12 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1173,7 +1221,7 @@
       <c r="B4" s="4">
         <v>44287</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
@@ -1306,9 +1354,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" ht="57.6" spans="1:10">
       <c r="A11">
         <v>1008</v>
+      </c>
+      <c r="B11" s="4">
+        <v>44349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44355</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:1">
@@ -1403,8 +1469,8 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1421,7 +1487,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1462,16 +1528,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1485,16 +1551,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1505,16 +1571,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1528,13 +1594,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1542,7 +1608,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="9" ht="72" spans="1:9">
+    <row r="9" ht="72" spans="1:10">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -1553,7 +1619,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1562,20 +1628,36 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>1007</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" ht="28.8" spans="1:9">
       <c r="A11">
         <v>1008</v>
+      </c>
+      <c r="B11" s="4">
+        <v>44349</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4">
+        <v>44355</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
New task 1010 and Previous Task 1008
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>UI development</t>
   </si>
@@ -115,31 +115,19 @@
     <t>1) Hide Column,Sort column,Move column,tooltip on column
 2) Get and Set Column width and order
 3) Export and Delete and Edit function 
-4) Working on dynamic pagination as discussed</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Reoderable,Tooltip,Export,Delete and Edit columnMenu properties and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+4) Working on dynamic pagination as discussed
+5) Add default CheckBox control beside Delete Button in current grid extender.
+6) Add a Property textbox which will take the number of columns which are not editable.    
+7) Add Filter option like selecting number of fields for search in.
+8) Given functionality for export all records to PDF/Excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reoderable,Tooltip,Export,Delete and Edit columnMenu properties and 
+Events like reorderColumn,resizeColumn,remove,save and dataBinding
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Events like reorderColumn,resizeColumn,remove,save and dataBinding</t>
-    </r>
+  </si>
+  <si>
+    <t>Listview Extender</t>
   </si>
   <si>
     <t>SQL development</t>
@@ -186,11 +174,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -221,8 +209,38 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -230,7 +248,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,107 +308,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,6 +368,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -392,79 +404,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,91 +548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,6 +559,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -592,17 +589,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,6 +610,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -633,15 +630,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,164 +662,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1160,11 +1145,11 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1221,7 +1206,7 @@
       <c r="B4" s="4">
         <v>44287</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
@@ -1354,7 +1339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" ht="57.6" spans="1:10">
+    <row r="11" ht="144" spans="1:10">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -1370,10 +1355,13 @@
       <c r="E11" s="4">
         <v>44355</v>
       </c>
+      <c r="F11" s="4">
+        <v>44363</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1382,9 +1370,18 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1010</v>
+      </c>
+      <c r="B13" s="4">
+        <v>44364</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -1487,7 +1484,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1528,16 +1525,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1551,16 +1548,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1571,16 +1568,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1594,13 +1591,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1619,7 +1616,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1628,16 +1625,16 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
         <v>1007</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="1:9">
@@ -1651,13 +1648,13 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4">
         <v>44355</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
Task 1010 First delivery
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>UI development</t>
   </si>
@@ -130,6 +130,12 @@
     <t>Listview Extender</t>
   </si>
   <si>
+    <t>1) Added New List Extender from database with properties and events
+2) Search functionality
+3) Sorting functionality
+4) Buttons like add,delete clone added</t>
+  </si>
+  <si>
     <t>SQL development</t>
   </si>
   <si>
@@ -174,11 +180,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -210,12 +216,42 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -225,45 +261,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,6 +291,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -293,61 +321,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,6 +374,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -380,144 +542,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -530,25 +554,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,9 +570,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,15 +590,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,6 +633,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -651,159 +659,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -814,7 +820,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1145,11 +1151,11 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1370,7 +1376,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" ht="72" spans="1:9">
       <c r="A13">
         <v>1010</v>
       </c>
@@ -1382,6 +1388,12 @@
       </c>
       <c r="D13" t="s">
         <v>11</v>
+      </c>
+      <c r="E13" s="4">
+        <v>44368</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:1">
@@ -1484,7 +1496,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1525,16 +1537,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1548,16 +1560,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1568,16 +1580,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1591,13 +1603,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1616,7 +1628,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1625,7 +1637,7 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1634,7 +1646,7 @@
         <v>1007</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="1:9">
@@ -1648,13 +1660,13 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="4">
         <v>44355</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
1008 - 3rd delivery and 1011 new task
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>UI development</t>
   </si>
@@ -119,7 +119,8 @@
 5) Add default CheckBox control beside Delete Button in current grid extender.
 6) Add a Property textbox which will take the number of columns which are not editable.    
 7) Add Filter option like selecting number of fields for search in.
-8) Given functionality for export all records to PDF/Excel</t>
+8) Given functionality for export all records to PDF/Excel
+9) Export checked records only</t>
   </si>
   <si>
     <t xml:space="preserve">Reoderable,Tooltip,Export,Delete and Edit columnMenu properties and 
@@ -134,6 +135,9 @@
 2) Search functionality
 3) Sorting functionality
 4) Buttons like add,delete clone added</t>
+  </si>
+  <si>
+    <t>SQL Solution and Services-UI devlopment</t>
   </si>
   <si>
     <t>SQL development</t>
@@ -180,11 +184,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -216,6 +220,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -223,7 +234,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,52 +242,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,6 +279,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -298,13 +294,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -329,6 +318,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -338,7 +341,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,8 +355,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,85 +378,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,97 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,17 +569,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -665,151 +658,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -820,7 +824,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1151,11 +1155,11 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1345,7 +1349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" ht="144" spans="1:10">
+    <row r="11" ht="158.4" spans="1:10">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -1363,6 +1367,9 @@
       </c>
       <c r="F11" s="4">
         <v>44363</v>
+      </c>
+      <c r="G11" s="4">
+        <v>44369</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>27</v>
@@ -1396,9 +1403,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>1011</v>
+      </c>
+      <c r="B14" s="4">
+        <v>44369</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1478,8 +1494,8 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1496,7 +1512,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1537,16 +1553,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1560,16 +1576,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1580,16 +1596,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1603,13 +1619,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1628,7 +1644,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1637,7 +1653,7 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1646,7 +1662,7 @@
         <v>1007</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="1:9">
@@ -1660,13 +1676,13 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="4">
         <v>44355</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
1011 update task detail
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="18468" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>UI development</t>
   </si>
@@ -140,6 +140,12 @@
     <t>SQL Solution and Services-UI devlopment</t>
   </si>
   <si>
+    <t>1) Add new control sidemenu with default facility
+2) API called for get all solution and services
+3) UI changes as described in the document
+4) Worked on feedback points like add click event for settings and help button,one solution should open at a time, click event for item selection, remove up-down icon.</t>
+  </si>
+  <si>
     <t>SQL development</t>
   </si>
   <si>
@@ -184,9 +190,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -219,6 +225,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -226,8 +248,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,32 +263,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,6 +325,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -319,14 +341,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,30 +356,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,73 +384,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,108 +565,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,6 +589,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,21 +656,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -672,7 +678,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -681,16 +690,13 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -699,121 +705,121 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1155,11 +1161,11 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1403,7 +1409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" ht="86.4" spans="1:9">
       <c r="A14">
         <v>1011</v>
       </c>
@@ -1415,6 +1421,12 @@
       </c>
       <c r="D14" t="s">
         <v>11</v>
+      </c>
+      <c r="E14" s="4">
+        <v>44375</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1512,7 +1524,7 @@
   <sheetData>
     <row r="1" ht="21" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1553,16 +1565,16 @@
         <v>44287</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" s="4">
         <v>44298</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -1576,16 +1588,16 @@
         <v>44307</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4">
         <v>44308</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:9">
@@ -1596,16 +1608,16 @@
         <v>44313</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4">
         <v>44315</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" ht="72" spans="1:9">
@@ -1619,13 +1631,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" s="4">
         <v>44326</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -1644,7 +1656,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="4">
         <v>44336</v>
@@ -1653,7 +1665,7 @@
         <v>44341</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1662,7 +1674,7 @@
         <v>1007</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="1:9">
@@ -1676,13 +1688,13 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" s="4">
         <v>44355</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:1">

</xml_diff>

<commit_message>
Task 1010 -task update with new reorder functionality
</commit_message>
<xml_diff>
--- a/DeliveryNotes/Managing Tasks.xlsx
+++ b/DeliveryNotes/Managing Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" activeTab="1"/>
+    <workbookView windowWidth="18468" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="3" r:id="rId1"/>
@@ -143,7 +143,9 @@
     <t>1) Add new control sidemenu with default facility
 2) API called for get all solution and services
 3) UI changes as described in the document
-4) Worked on feedback points like add click event for settings and help button,one solution should open at a time, click event for item selection, remove up-down icon.</t>
+4) Worked on feedback points like add click event for settings and help button,one solution should open at a time, click event for item selection, remove up-down icon.
+5) Add reorder button
+6) open popup with defied functionality like sort services,hide icons,save to DB functionality.</t>
   </si>
   <si>
     <t>SQL development</t>
@@ -214,10 +216,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="23">
@@ -249,6 +251,142 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,142 +394,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -408,187 +410,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,22 +604,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,26 +643,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,6 +667,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -699,151 +690,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1184,24 +1186,24 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.42857142857143" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="40.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="17.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="9.42592592592593" customWidth="1"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="40.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="17.287037037037" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="7" width="10.2857142857143" customWidth="1"/>
-    <col min="9" max="9" width="53.8571428571429" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7142857142857" customWidth="1"/>
+    <col min="6" max="7" width="10.287037037037" customWidth="1"/>
+    <col min="9" max="9" width="53.8611111111111" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:1">
@@ -1239,7 +1241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="45" spans="1:10">
+    <row r="4" ht="43.2" spans="1:10">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -1262,7 +1264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" ht="60" spans="1:9">
+    <row r="5" ht="57.6" spans="1:9">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -1290,7 +1292,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="75" spans="1:10">
+    <row r="7" ht="57.6" spans="1:10">
       <c r="A7">
         <v>1004</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" ht="60" spans="1:9">
+    <row r="8" ht="57.6" spans="1:9">
       <c r="A8">
         <v>1005</v>
       </c>
@@ -1333,7 +1335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="105" spans="1:9">
+    <row r="9" ht="86.4" spans="1:9">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" ht="60" spans="1:9">
+    <row r="10" ht="43.2" spans="1:9">
       <c r="A10">
         <v>1007</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" ht="195" spans="1:10">
+    <row r="11" ht="158.4" spans="1:10">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -1413,7 +1415,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="13" ht="75" spans="1:9">
+    <row r="13" ht="72" spans="1:9">
       <c r="A13">
         <v>1010</v>
       </c>
@@ -1433,7 +1435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" ht="90" spans="1:9">
+    <row r="14" ht="129.6" spans="1:9">
       <c r="A14">
         <v>1011</v>
       </c>
@@ -1448,6 +1450,9 @@
       </c>
       <c r="E14" s="4">
         <v>44375</v>
+      </c>
+      <c r="F14" s="4">
+        <v>44378</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>32</v>
@@ -1530,20 +1535,20 @@
   <sheetPr/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.42857142857143" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="51.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="16.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="19.4285714285714" customWidth="1"/>
-    <col min="6" max="7" width="10.2857142857143" customWidth="1"/>
-    <col min="9" max="9" width="53.8571428571429" style="1" customWidth="1"/>
-    <col min="10" max="10" width="53.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="9.42592592592593" customWidth="1"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="51.1388888888889" customWidth="1"/>
+    <col min="4" max="4" width="16.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="19.4259259259259" customWidth="1"/>
+    <col min="6" max="7" width="10.287037037037" customWidth="1"/>
+    <col min="9" max="9" width="53.8611111111111" style="1" customWidth="1"/>
+    <col min="10" max="10" width="53.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:1">
@@ -1581,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="75" spans="1:10">
+    <row r="4" ht="72" spans="1:10">
       <c r="A4">
         <v>1001</v>
       </c>
@@ -1604,7 +1609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" ht="30" spans="1:9">
+    <row r="5" ht="28.8" spans="1:9">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -1624,7 +1629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" ht="60" spans="1:9">
+    <row r="6" ht="57.6" spans="1:9">
       <c r="A6">
         <v>1003</v>
       </c>
@@ -1644,7 +1649,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" ht="75" spans="1:9">
+    <row r="7" ht="72" spans="1:9">
       <c r="A7">
         <v>1004</v>
       </c>
@@ -1669,7 +1674,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="9" ht="90" spans="1:10">
+    <row r="9" ht="72" spans="1:10">
       <c r="A9">
         <v>1006</v>
       </c>
@@ -1701,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" ht="30" spans="1:9">
+    <row r="11" ht="28.8" spans="1:9">
       <c r="A11">
         <v>1008</v>
       </c>
@@ -1721,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" ht="120" spans="1:10">
+    <row r="12" ht="115.2" spans="1:10">
       <c r="A12">
         <v>1009</v>
       </c>
@@ -1752,7 +1757,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="14" ht="75" spans="1:9">
+    <row r="14" ht="57.6" spans="1:9">
       <c r="A14">
         <v>1011</v>
       </c>

</xml_diff>